<commit_message>
Commting IVR call trace report changes
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/IVRCallTraceReportData.xlsx
+++ b/ocms/src/test/resources/TestData/IVRCallTraceReportData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3AAF32-E090-41C9-9012-987970631C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15195" windowHeight="6495" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,6 @@
     <sheet name="Queries" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="58">
   <si>
     <t>Report Channel</t>
   </si>
@@ -95,18 +95,12 @@
     <t>UCID</t>
   </si>
   <si>
-    <t>10000003601590600000</t>
-  </si>
-  <si>
     <t>90</t>
   </si>
   <si>
     <t>Caller ID</t>
   </si>
   <si>
-    <t>40021</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -128,12 +122,6 @@
     <t xml:space="preserve">Ends with </t>
   </si>
   <si>
-    <t>Identification</t>
-  </si>
-  <si>
-    <t>S1234567A</t>
-  </si>
-  <si>
     <t>40034</t>
   </si>
   <si>
@@ -141,12 +129,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>242</t>
-  </si>
-  <si>
-    <t>S21</t>
   </si>
   <si>
     <t>Deleted</t>
@@ -185,11 +167,65 @@
 GROUP BY [Menu],[CallerID] ORDER BY CallerID ASC;
 </t>
   </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Does not contain</t>
+  </si>
+  <si>
+    <t>Hotline Number</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Is greater than or equal</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10000003611590646420</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Is not equal to</t>
+  </si>
+  <si>
+    <t>40021</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Caller Status</t>
+  </si>
+  <si>
+    <t>Starts With</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ends With</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,29 +540,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +575,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -552,6 +591,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -561,25 +603,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -608,10 +651,10 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,22 +671,22 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -660,19 +703,19 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -689,103 +732,132 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
       </c>
       <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -794,21 +866,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,8 +893,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -834,6 +909,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -842,22 +920,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,8 +952,11 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -889,6 +971,9 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -897,22 +982,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,8 +1011,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -938,6 +1027,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -946,22 +1038,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1069,11 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -993,6 +1088,9 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1001,25 +1099,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
+    <col min="9" max="9" width="29.81640625" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1080,13 +1178,13 @@
         <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1106,16 +1204,164 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1124,23 +1370,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,13 +1403,13 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1177,13 +1423,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting changes of email reports
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/IVRCallTraceReportData.xlsx
+++ b/ocms/src/test/resources/TestData/IVRCallTraceReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE1820-4636-49CB-8703-9B8E2BDD19B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2BFFCA-6E1A-4903-BE08-E33D51313F73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="64">
   <si>
     <t>Report Channel</t>
   </si>
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>DB Type</t>
+  </si>
+  <si>
+    <t>MS SQL</t>
+  </si>
+  <si>
+    <t>MYSQL</t>
+  </si>
+  <si>
+    <t>01-06-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>07-06-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>Select * from AGT_Agent_TimeTrack;</t>
   </si>
 </sst>
 </file>
@@ -1371,64 +1389,98 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.81640625" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="406" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>